<commit_message>
fix bug on rekap nilai
</commit_message>
<xml_diff>
--- a/public/uploads/rekap-nilai.xlsx
+++ b/public/uploads/rekap-nilai.xlsx
@@ -4,31 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="XII SIJA 2" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="XI BC 1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Ujian</t>
   </si>
   <si>
-    <t>Contoh ujian 40 soal</t>
+    <t>SIMULASI PTS KELAS XI</t>
   </si>
   <si>
     <t>Tanggal</t>
   </si>
   <si>
-    <t>Senin 01 Maret 2021 10:46 - 11:26</t>
+    <t>Kamis 04 Maret 2021 09:00 - 10:00</t>
   </si>
   <si>
     <t>Durasi</t>
   </si>
   <si>
-    <t>40 menit</t>
+    <t>60 menit</t>
   </si>
   <si>
     <t>KKM</t>
@@ -46,106 +46,112 @@
     <t>Nilai Total</t>
   </si>
   <si>
-    <t>AHMAD AKBAR ALLAYA</t>
-  </si>
-  <si>
-    <t>AILSA NAURAH SUKMONO</t>
-  </si>
-  <si>
-    <t>ACHMAD KURNIA ILHAM</t>
-  </si>
-  <si>
-    <t>ANNISA SYAHARANI</t>
-  </si>
-  <si>
-    <t>AZMITA PUTRI SHERLIAN</t>
-  </si>
-  <si>
-    <t>BENIKI PANJI BATHI</t>
-  </si>
-  <si>
-    <t>ARIEL SHARON FERDINANDUS</t>
-  </si>
-  <si>
-    <t>DAFFA PERMANA</t>
-  </si>
-  <si>
-    <t>Fikri Akbar Pramudya</t>
-  </si>
-  <si>
-    <t>GALUH FIKRY MAULANA AHCMAD</t>
-  </si>
-  <si>
-    <t>ARINDA AURA OKTAVIANI</t>
-  </si>
-  <si>
-    <t>ILHAM FAJRIANSYAH</t>
-  </si>
-  <si>
-    <t>AULIYA RAHMAWATI</t>
-  </si>
-  <si>
-    <t>GHULAM DIAS ABBIYU</t>
-  </si>
-  <si>
-    <t>ILYAS MUBARROK</t>
-  </si>
-  <si>
-    <t>Mohammad Dika Rifa Nadi</t>
-  </si>
-  <si>
-    <t>MUHAMAD RIZKY ARMANTO</t>
-  </si>
-  <si>
-    <t>MAULINA</t>
-  </si>
-  <si>
-    <t>JULIANO FAKHRI</t>
-  </si>
-  <si>
-    <t>MUHAMMAD IKHSAN DWI EFENDI</t>
-  </si>
-  <si>
-    <t>MUHAMMAD DURMUJI</t>
-  </si>
-  <si>
-    <t>MUHAMMAD SAIFUL MIQDAR</t>
-  </si>
-  <si>
-    <t>MUHAMMAD ZAKI REVANDI</t>
-  </si>
-  <si>
-    <t>SANTI ELISHABET</t>
-  </si>
-  <si>
-    <t>SAZA FADILAH</t>
-  </si>
-  <si>
-    <t>MUKHLIS</t>
-  </si>
-  <si>
-    <t>NAWANG NOVANTI LISTYANINGSIH</t>
-  </si>
-  <si>
-    <t>SEKA ABDUL MATIN</t>
-  </si>
-  <si>
-    <t>RANDY YULIANO</t>
-  </si>
-  <si>
-    <t>WIRA PRADIPA ARYAPUTRA</t>
-  </si>
-  <si>
-    <t>VEYDAYEN FATZLA AL FIANSYACH</t>
-  </si>
-  <si>
-    <t>TAUFIQURRAHMAN</t>
-  </si>
-  <si>
-    <t>YASSIN DWI CAHYO</t>
-  </si>
-  <si>
-    <t>MUHAMMAD ALIF DZAKY AMMAR</t>
+    <t>AMIRAH NUR AINI</t>
+  </si>
+  <si>
+    <t>ANGEL LYKA SARI</t>
+  </si>
+  <si>
+    <t>Ayu Yuliana</t>
+  </si>
+  <si>
+    <t>AINI PUTRI AZIZAH</t>
+  </si>
+  <si>
+    <t>Alief Randhinka Putra</t>
+  </si>
+  <si>
+    <t>Arya Juliyawan</t>
+  </si>
+  <si>
+    <t>Aditya Rafly Fatahhudin</t>
+  </si>
+  <si>
+    <t>ABDUL RAHMAN</t>
+  </si>
+  <si>
+    <t>ANDI RADITA DAFA</t>
+  </si>
+  <si>
+    <t>ANISA PURI APRILIA</t>
+  </si>
+  <si>
+    <t>Chika Yuliani</t>
+  </si>
+  <si>
+    <t>INTAN RAMADHANIA</t>
+  </si>
+  <si>
+    <t>INTAN NURAINI</t>
+  </si>
+  <si>
+    <t>DWI RIYANTO</t>
+  </si>
+  <si>
+    <t>DINA NOVIA PUTRI</t>
+  </si>
+  <si>
+    <t>Fikri Hawari</t>
+  </si>
+  <si>
+    <t>FASHA RIANI PUTRI</t>
+  </si>
+  <si>
+    <t>JUANDA</t>
+  </si>
+  <si>
+    <t>DEFIRA ARYANTI</t>
+  </si>
+  <si>
+    <t>MUTIARA PUTRI AZZAHRA</t>
+  </si>
+  <si>
+    <t>NUR FARIZ DIRJA</t>
+  </si>
+  <si>
+    <t>Hilda Al Kayis</t>
+  </si>
+  <si>
+    <t>Iip Dany Budi Utomo</t>
+  </si>
+  <si>
+    <t>NABILAH HARSIKA</t>
+  </si>
+  <si>
+    <t>PITRIA</t>
+  </si>
+  <si>
+    <t>Neng Silvi Aprilianti</t>
+  </si>
+  <si>
+    <t>MUHAMMAD KHALIL FERGAL</t>
+  </si>
+  <si>
+    <t>Muhammad Fadhil Nur Iskandar</t>
+  </si>
+  <si>
+    <t>MUHAMAD KEVIN</t>
+  </si>
+  <si>
+    <t>PUTRI SALSABILLA</t>
+  </si>
+  <si>
+    <t>Rara Safira</t>
+  </si>
+  <si>
+    <t>WINIE LAILATUL RHAMADANTI WIBOWO</t>
+  </si>
+  <si>
+    <t>Sofi Dwiyanti</t>
+  </si>
+  <si>
+    <t>Siska Audina Fadilah</t>
+  </si>
+  <si>
+    <t>SYIFA FADILLAH</t>
+  </si>
+  <si>
+    <t>Viona</t>
   </si>
 </sst>
 </file>
@@ -522,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -572,13 +578,13 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,13 +592,13 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,13 +606,13 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,13 +620,13 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,13 +634,13 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,13 +648,13 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,13 +662,13 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,13 +676,13 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -684,13 +690,13 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,13 +704,13 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,13 +718,13 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,13 +732,13 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,13 +746,13 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,13 +760,13 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,13 +774,13 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,13 +788,13 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,13 +802,13 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,13 +816,13 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,13 +830,13 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,13 +844,13 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -852,13 +858,13 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,13 +872,13 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,13 +886,13 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -894,13 +900,13 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,13 +914,13 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,13 +928,13 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,13 +942,13 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,13 +956,13 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,13 +970,13 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,13 +984,13 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -992,13 +998,13 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1006,13 +1012,13 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,13 +1026,13 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,13 +1040,41 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>14</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>64</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>